<commit_message>
remmoved notes from designPatterns
</commit_message>
<xml_diff>
--- a/RunningNotes.xlsx
+++ b/RunningNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="857" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="857" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Collection" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="158">
   <si>
     <t>Topic</t>
   </si>
@@ -828,6 +828,87 @@
   </si>
   <si>
     <t>Binary</t>
+  </si>
+  <si>
+    <t>Chain of Responsibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interpreter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mediator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Momento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strategy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visitor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adapter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decorator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flyweight </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Factory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstract Factory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Builder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototype </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singleton </t>
+  </si>
+  <si>
+    <t>Creational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structural </t>
+  </si>
+  <si>
+    <t>Behavioral </t>
+  </si>
+  <si>
+    <t>Gives several algorithms that can be used to perform particular operation or task</t>
   </si>
 </sst>
 </file>
@@ -968,7 +1049,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1025,6 +1106,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1309,7 +1396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1778,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2116,13 +2203,157 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.53125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.53125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.06640625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B3" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B17" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B19" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B20" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B21" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B22" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B25" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B26" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B27" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B28" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B29" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Quick sort and thread started
</commit_message>
<xml_diff>
--- a/RunningNotes.xlsx
+++ b/RunningNotes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="857" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="857" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Collection" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Java" sheetId="8" r:id="rId7"/>
     <sheet name="DesignPattern" sheetId="3" r:id="rId8"/>
     <sheet name="DesignPriniciples" sheetId="5" r:id="rId9"/>
-    <sheet name="TO.DO" sheetId="7" r:id="rId10"/>
+    <sheet name="Topic" sheetId="7" r:id="rId10"/>
     <sheet name="Thread" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="202">
   <si>
     <t>Topic</t>
   </si>
@@ -63,11 +63,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>The ability to inspect the code in the system and see object types is not reflection, but rather Type Introspection. 
-Reflection is then the ability to make modifications at runtime by making use of introspection. 
-The distinction is necessary here as some languages support introspection, but do not support reflection. One such example is C++</t>
   </si>
   <si>
     <t>Reflection</t>
@@ -309,14 +304,6 @@
     </r>
   </si>
   <si>
-    <t>class Entry&lt;K,V&gt; extends HashMap.Node&lt;K,V&gt; {
-    Entry&lt;K,V&gt; before, after;
-    Entry(int hash, K key, V value, Node&lt;K,V&gt; next) {
-        super(hash, key, value, next);
-    }
-}</t>
-  </si>
-  <si>
     <t>*OverComes the drawback of HashMap by maintaing the insertion order using two added pointers.
 *It maintains a 3rd arguments , if set to true, the least accessed element is listed first.</t>
   </si>
@@ -339,11 +326,6 @@
     <t>Hashtable</t>
   </si>
   <si>
-    <t>*Sorted, by natural ordered or by comparator.
-*Does not take null, because it needs to compare while putting.
-*The head of the queue is the least element based on the ordering.</t>
-  </si>
-  <si>
     <t>Data Structure</t>
   </si>
   <si>
@@ -353,9 +335,6 @@
     <t>Data Structures</t>
   </si>
   <si>
-    <t>MultiThreading</t>
-  </si>
-  <si>
     <t>Java Memory Management</t>
   </si>
   <si>
@@ -365,9 +344,6 @@
     <t>Interview Puzzle</t>
   </si>
   <si>
-    <t>JVM</t>
-  </si>
-  <si>
     <t>Executor framework</t>
   </si>
   <si>
@@ -386,20 +362,10 @@
     <t>Data structure is a particular way of organizing and storing data in a computer so that it can be accessed and modified efficiently. More precisely, a data structure is a collection of data values, the relationships among them, and the functions or operations that can be applied to the data.</t>
   </si>
   <si>
-    <t xml:space="preserve">HashSet uses the functionality of HashMap like put &amp; get. It constructs a new HashMap whenever a new hashSet is created.
-LinkedHasHashMap extends HashMap function(insertion order)  </t>
-  </si>
-  <si>
     <t>Build Management ANT/Maven</t>
   </si>
   <si>
     <t xml:space="preserve">Design Patterns </t>
-  </si>
-  <si>
-    <t>Principles</t>
-  </si>
-  <si>
-    <t>Algorithms</t>
   </si>
   <si>
     <r>
@@ -720,30 +686,15 @@
     <t>Quicksort</t>
   </si>
   <si>
-    <t>O(n^2)</t>
-  </si>
-  <si>
-    <t>O(log(n))</t>
-  </si>
-  <si>
     <t>Mergesort</t>
   </si>
   <si>
-    <t>O(n log(n))</t>
-  </si>
-  <si>
-    <t>O(n)</t>
-  </si>
-  <si>
     <t>Timsort</t>
   </si>
   <si>
     <t>Heapsort</t>
   </si>
   <si>
-    <t>O(1)</t>
-  </si>
-  <si>
     <t>Bubble Sort</t>
   </si>
   <si>
@@ -759,25 +710,13 @@
     <t>Shell Sort</t>
   </si>
   <si>
-    <t>O(n(log(n))^2)</t>
-  </si>
-  <si>
     <t>Bucket Sort</t>
   </si>
   <si>
     <t>Radix Sort</t>
   </si>
   <si>
-    <t>O(nk)</t>
-  </si>
-  <si>
-    <t>O(n+k)</t>
-  </si>
-  <si>
     <t>Counting Sort</t>
-  </si>
-  <si>
-    <t>O(k)</t>
   </si>
   <si>
     <t>Cubesort</t>
@@ -906,9 +845,6 @@
     <t>Behavioral </t>
   </si>
   <si>
-    <t>Gives several algorithms that can be used to perform particular operation or task</t>
-  </si>
-  <si>
     <t>Java architecture</t>
   </si>
   <si>
@@ -1146,12 +1082,304 @@
 For web server delay is negligible when compared to network delays but for interactive graphics delay is high priority so more memory is used to reduce the frequency of GC.</t>
     </r>
   </si>
+  <si>
+    <t>Gives several types algorithms that can be used to perform particular operation or task</t>
+  </si>
+  <si>
+    <t>HackerRank</t>
+  </si>
+  <si>
+    <t>Searching</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Design Principles</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Architecture and JVM </t>
+  </si>
+  <si>
+    <t>Reflection is then the ability to make modifications at runtime by making use of introspection. 
+The distinction is necessary here as some languages support introspection, but do not support reflection. One such example is C++</t>
+  </si>
+  <si>
+    <t>The ability to inspect the code in the system and see object types is not reflection, but rather Type Introspection.</t>
+  </si>
+  <si>
+    <t>Single responsibility</t>
+  </si>
+  <si>
+    <t>look for all the reasons a class has to change. If there is more than one reason to change a class then it means this class does not follow the single responsibility principle.
+Low coupling and high cohesion.</t>
+  </si>
+  <si>
+    <t>Open-Closed Principle</t>
+  </si>
+  <si>
+    <t>open-closed-principle</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Design Pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Command Pattern</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>This priniciple is more related to the controller class. 
+The class exhibits its extenable functionality by providing a defined protocol(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Interface/Composition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) instead of adding swithCase/if-else or inheriting/modifining .
+If any functionality (method) depends on only primary properties we can declare them in the interface.If a functionality depends on an external entity, always use composition rather than inheritance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Chrome browser. It can take any number of extension. The chrome app does not need any modificaton but can do more things by adding extensions.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Design Pattern </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:Factory Method and Abstract Factory
+This will make sure old implementation is not disturbed and also avoids wired bugs
+Lean/tends towards Interface</t>
+    </r>
+  </si>
+  <si>
+    <t>Liskov Substitution Principle</t>
+  </si>
+  <si>
+    <t>Principle states that any method that takes class X as a parameter must be able to work with any subclasses of X.
+The principle makes sure that every class follows the contract defined by its parent class.</t>
+  </si>
+  <si>
+    <t>Lean/tends towards inheritance. 
+Does it ?</t>
+  </si>
+  <si>
+    <t>Dependency Inversion Principle</t>
+  </si>
+  <si>
+    <t>Interface Segregation Principle</t>
+  </si>
+  <si>
+    <t>Clients should not be forced to depend upon the interfaces that they do not use.</t>
+  </si>
+  <si>
+    <t>Program to an interface, not to an implementation.</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class Entry&lt;K,V&gt; extends HashMap.Node&lt;K,V&gt; {
+    Entry&lt;K,V&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>before, after</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+    Entry(int hash, K key, V value, Node&lt;K,V&gt; next) {
+        super(hash, key, value, next);
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedHasHashMap extends HashMap function(insertion order)  </t>
+  </si>
+  <si>
+    <t>HashSet uses the functionality of HashMap like put &amp; get. It constructs a new HashMap whenever a new hashSet is created</t>
+  </si>
+  <si>
+    <t>HashSet</t>
+  </si>
+  <si>
+    <t>LinkedHasHashMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set returns true to indicate that the object is added into the map.
+return map.put(e, PRESENT)==null;
+</t>
+  </si>
+  <si>
+    <t>*Using Queue API we get Sorted, by natural ordered or by comparator.
+*Does not take null, because it needs to compare while putting.
+*The head of the queue is the least element based on the ordering.</t>
+  </si>
+  <si>
+    <t>Design Pattern is a template that has to be implemented to handle a problem</t>
+  </si>
+  <si>
+    <t>Design Pattern</t>
+  </si>
+  <si>
+    <t>Behavioral patterns are used in communications between entities and make it easier and more flexible for these entities to communicate.</t>
+  </si>
+  <si>
+    <t>Constructs complex objects using step-by-step approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Creates families of related dependent objects</t>
+  </si>
+  <si>
+    <t>Creates objects of several related classes without specifying the exact object to be created</t>
+  </si>
+  <si>
+    <t>Ensures that at most only one instance of an object exists throughout application</t>
+  </si>
+  <si>
+    <t>Class Loader</t>
+  </si>
+  <si>
+    <t>These design patterns are all about Class and Object composition. Structural object-patterns define ways to compose objects to obtain new functionality.</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>It provides an alternative for inhertance
+Single Responsibility Principle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n(log(n))^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n log(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n+k</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n+k </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> k </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> log  n  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> n^2 or nlogn(randomize)</t>
+  </si>
+  <si>
+    <t>Maintainable &amp; Expandable
+Clean &amp; Readable</t>
+  </si>
+  <si>
+    <t>this pattern allows responsibilities to be added to an object</t>
+  </si>
+  <si>
+    <t>How randomized pivot reduce the complexity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1182,8 +1410,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1202,8 +1437,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1267,25 +1508,16 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <bottom style="thin">
         <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1304,15 +1536,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1338,17 +1561,37 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1630,9 +1873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1655,59 +1900,59 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -1715,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1723,50 +1968,50 @@
     </row>
     <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="299.25" x14ac:dyDescent="0.45">
@@ -1774,31 +2019,50 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1809,114 +2073,145 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="13"/>
+    <col min="3" max="3" width="9.06640625" style="10"/>
+    <col min="6" max="6" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="13">
+        <v>48</v>
+      </c>
+      <c r="C2" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="13">
+        <v>49</v>
+      </c>
+      <c r="C3" s="10">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="13">
+        <v>50</v>
+      </c>
+      <c r="C4" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>150</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>50</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>187</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F17:G19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1936,12 +2231,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1954,28 +2249,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="13.59765625" style="9" customWidth="1"/>
     <col min="2" max="3" width="74.59765625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11"/>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1986,57 +2281,60 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
-        <v>19</v>
+      <c r="A3" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>10</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
-        <v>91</v>
+      <c r="A5" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
-        <v>55</v>
+      <c r="A6" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
-        <v>160</v>
+      <c r="A7" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="384.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
-        <v>56</v>
+      <c r="A8" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2050,17 +2348,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="14"/>
+    <col min="1" max="1" width="9.06640625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
-        <v>129</v>
+      <c r="A1" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2074,57 +2372,60 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.53125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.53125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83.73046875" style="1" customWidth="1"/>
     <col min="3" max="3" width="65.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+    <row r="1" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="15" t="s">
-        <v>95</v>
+      <c r="A3" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="15" t="s">
-        <v>124</v>
+      <c r="A4" s="12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="15" t="s">
-        <v>125</v>
+      <c r="A5" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>126</v>
+      <c r="A6" s="12" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="15" t="s">
-        <v>127</v>
+      <c r="A7" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="15" t="s">
-        <v>128</v>
+      <c r="A8" s="12" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2135,184 +2436,193 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="14" customFormat="1" ht="27.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>121</v>
+    <row r="1" spans="1:3" s="11" customFormat="1" ht="27.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="16"/>
+      <c r="B2" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>99</v>
+      <c r="A3" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s">
-        <v>101</v>
+        <v>190</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>102</v>
+      <c r="A4" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>101</v>
+        <v>190</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>103</v>
+      <c r="A5" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
+        <v>190</v>
+      </c>
+      <c r="C5" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
+      <c r="A6" s="11"/>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>105</v>
+      <c r="A7" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" t="s">
-        <v>104</v>
+        <v>198</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>106</v>
+      <c r="A8" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>104</v>
+        <v>191</v>
+      </c>
+      <c r="C8" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>107</v>
+      <c r="A9" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
+        <v>191</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>108</v>
+      <c r="A10" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" t="s">
-        <v>101</v>
+        <v>191</v>
+      </c>
+      <c r="C10" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" t="s">
-        <v>101</v>
-      </c>
+      <c r="A11" s="11"/>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" t="s">
-        <v>104</v>
+        <v>191</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>114</v>
+        <v>191</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C14" t="s">
-        <v>116</v>
+        <v>189</v>
+      </c>
+      <c r="C14" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>100</v>
       </c>
-      <c r="C15" t="s">
-        <v>101</v>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2326,77 +2636,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="144.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
-        <v>44</v>
+      <c r="A1" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
-        <v>19</v>
+      <c r="A2" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="9" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="12" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2407,72 +2717,77 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="146.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.59765625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" style="7" customWidth="1"/>
     <col min="2" max="2" width="145.33203125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="146.73046875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
-        <v>64</v>
+      <c r="A1" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="10" t="s">
-        <v>70</v>
+      <c r="A2" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="10" t="s">
-        <v>69</v>
+      <c r="A3" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="10" t="s">
-        <v>72</v>
+      <c r="A8" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
-        <v>67</v>
+      <c r="A10" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="10" t="s">
-        <v>157</v>
+      <c r="A12" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2483,7 +2798,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -2491,144 +2806,185 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.53125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.1328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.53125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="22"/>
+    <col min="5" max="16384" width="9.06640625" style="17"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B3" s="23" t="s">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B5" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B18" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B21" s="18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B22" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="23" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="23" t="s">
+    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="23" t="s">
+      <c r="C25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="9" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B8" s="23" t="s">
+      <c r="C27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B9" s="23" t="s">
+      <c r="C28" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="18" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B10" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B11" s="23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B20" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B22" s="23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B25" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B26" s="23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B27" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B28" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B29" s="23" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2639,12 +2995,71 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.9296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="65.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="77.46484375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="114" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed files and added the content to Running Notes
</commit_message>
<xml_diff>
--- a/RunningNotes.xlsx
+++ b/RunningNotes.xlsx
@@ -3,28 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF71C02-CA9D-43FF-8B1E-4FDD28F66F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134C6342-91CC-4746-945C-E3CAF48CA6A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="936" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="936" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue" sheetId="18" r:id="rId1"/>
     <sheet name="Topics" sheetId="7" r:id="rId2"/>
-    <sheet name="Question" sheetId="14" r:id="rId3"/>
-    <sheet name="Puzzles" sheetId="19" r:id="rId4"/>
-    <sheet name="Collection" sheetId="1" r:id="rId5"/>
-    <sheet name="Concepts" sheetId="2" r:id="rId6"/>
-    <sheet name="Data Structures" sheetId="13" r:id="rId7"/>
-    <sheet name="Searching" sheetId="9" r:id="rId8"/>
-    <sheet name="Sorting" sheetId="10" r:id="rId9"/>
-    <sheet name="Complexity" sheetId="11" r:id="rId10"/>
-    <sheet name="Definition" sheetId="6" r:id="rId11"/>
-    <sheet name="Java" sheetId="8" r:id="rId12"/>
-    <sheet name="Software Architecture" sheetId="16" r:id="rId13"/>
-    <sheet name="Design Pattern" sheetId="3" r:id="rId14"/>
-    <sheet name="Design Priniciples" sheetId="5" r:id="rId15"/>
-    <sheet name="Java Versions" sheetId="17" r:id="rId16"/>
-    <sheet name="Thread" sheetId="12" r:id="rId17"/>
+    <sheet name="Git" sheetId="20" r:id="rId3"/>
+    <sheet name="Question" sheetId="14" r:id="rId4"/>
+    <sheet name="Puzzles" sheetId="19" r:id="rId5"/>
+    <sheet name="Collection" sheetId="1" r:id="rId6"/>
+    <sheet name="Concepts" sheetId="2" r:id="rId7"/>
+    <sheet name="Data Structures" sheetId="13" r:id="rId8"/>
+    <sheet name="Searching" sheetId="9" r:id="rId9"/>
+    <sheet name="Sorting" sheetId="10" r:id="rId10"/>
+    <sheet name="Complexity" sheetId="11" r:id="rId11"/>
+    <sheet name="Definition" sheetId="6" r:id="rId12"/>
+    <sheet name="Java" sheetId="8" r:id="rId13"/>
+    <sheet name="Software Architecture" sheetId="16" r:id="rId14"/>
+    <sheet name="Design Pattern" sheetId="3" r:id="rId15"/>
+    <sheet name="Design Priniciples" sheetId="5" r:id="rId16"/>
+    <sheet name="Java Versions" sheetId="17" r:id="rId17"/>
+    <sheet name="Thread" sheetId="12" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="344">
   <si>
     <t>Topic</t>
   </si>
@@ -2399,6 +2400,89 @@
   <si>
     <t>Chain of Responsi
 bility</t>
+  </si>
+  <si>
+    <t>----&gt;&gt;What is the complexity of recursive left shift operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">----&gt;&gt;prime number with root n complexity </t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/2307283/what-does-olog-n-mean-exactlyIn
+ In logarithm graph time curve decelerates as n increases.
+Logarithm is essentially the inverse of exponentiation.
+Now, if you can prove, that at every iteration of your algorithm you cut off a fraction of this space,
+ that is no less than some limit, this means that your algorithm is running in O(logN) time.
+O(log n) running times are very common in any sort of divide-and-conquer application, because you are (ideally) cutting the work in half every time.
+Then why not log(N/2)</t>
+  </si>
+  <si>
+    <t>1. Sort methodsd in collection
+2. add() addAll() 
+3. remove() removeALL() 
+4. Retain() clear()
+5. For loop in collection
+6. NavigationSet, NavigationMap</t>
+  </si>
+  <si>
+    <t>Iterator vs Iterable ; because iterable classes return Iterator object using the Iterator().</t>
+  </si>
+  <si>
+    <t>Collection col = new HashSet()	is better than	HashSet set = new Hashset() because we should code to the interface.
+But what if, i want to use the methods that are declared and defined in HashSet
+Answer : Type Cast works.</t>
+  </si>
+  <si>
+    <t>Branch
+***********
+$ git branch -d branch_name
+$ git branch -D branch_name
+$ git push origin --delete &lt;branch_name&gt;
+deletes the remote branch</t>
+  </si>
+  <si>
+    <t>First, you need to create your branch locally
+git checkout -b your_branch
+After that, you can work locally in your branch, when you are ready to share the branch, push it. 
+The next command pushes the branch to the remote repository origin and tracks it.
+git push -origin your_branch
+Your Teammates/colleagues can push to your branch by doing commits and then push explicitly
+... work ...
+git commit
+... work ...
+git commit
+git push origin HEAD:refs/heads/warRoom</t>
+  </si>
+  <si>
+    <t>If we push the changes to a &lt;branch&gt; using "-u" , then all your future pushes will be done to that &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>Revisit
+https://git-scm.com/book/en/v2/Git-Basics-Working-with-Remotes
+	:Showing Your Remotes
+$ git remote
+origin
+To see which remote servers you have configured, you can run the git remote command.It lists the shortnames of each remote handle you’ve specified.
+If you’ve cloned your repository, you should at least see origin,that is the default name Git gives to the server you cloned from.
+$ git remote -v
+origin  https://github.com/JamesTharakan/cognitiveLearning.git (fetch)
+origin  https://github.com/JamesTharakan/cognitiveLearning.git (push)
+shows you the URLs that Git has stored for the shortname(origin) to be used when reading and writing to that remote</t>
+  </si>
+  <si>
+    <t>git reset HEAD &lt;filePath&gt;
+git log --branches --not --remotes=origin
+Shows all commits that are in any of local branches but not in any of remote-tracking branches for origin
+ (what you have that origin doesn’t).
+git checkout -b branchname origin/branchname
+Here, by default we are setting the upstream branch, so you will not be facing the mentioned issue.</t>
+  </si>
+  <si>
+    <t>GC
+continued</t>
+  </si>
+  <si>
+    <t>Automatic Garbage collection is a process of looking at the Heap memory, identifying(also known as “marking”) the unreachable objects, and destroying(Sweep) them with compaction. An issue with this approach is that, as the number of objects increases, the Garbage Collection time keeps on increasing, as it needs to go through the entire list of objects, looking for the unreachable object.Since most of the objects are short-lived the Heap space is divided into generations like Young Generation, Old or Tenured Generation, and Permanent Generation.</t>
   </si>
 </sst>
 </file>
@@ -2642,9 +2726,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2659,17 +2740,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2958,7 +3042,7 @@
   <dimension ref="A3:A18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3071,6 +3155,81 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.53125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.73046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="3" spans="1:3" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Catalogue!A1" display="Sorting" xr:uid="{3267D2FA-DC3A-41D3-A13F-612768D8DED2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -3097,7 +3256,7 @@
       <c r="C1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="36"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -3111,7 +3270,7 @@
       <c r="E2" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="F2" s="36"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -3124,10 +3283,10 @@
       <c r="C3" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>287</v>
       </c>
     </row>
@@ -3141,10 +3300,10 @@
       <c r="C4" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3158,18 +3317,18 @@
       <c r="C5" s="25">
         <v>1</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="F5" s="38"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="11"/>
       <c r="C6" s="25"/>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>280</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3183,10 +3342,10 @@
       <c r="C7" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="36" t="s">
         <v>281</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3200,10 +3359,10 @@
       <c r="C8" s="25">
         <v>1</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="F8" s="38"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="24" t="s">
@@ -3215,10 +3374,10 @@
       <c r="C9" s="25">
         <v>1</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="38"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="24" t="s">
@@ -3230,18 +3389,18 @@
       <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="F10" s="38"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11"/>
       <c r="C11" s="25"/>
-      <c r="E11" s="37" t="s">
+      <c r="E11" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
@@ -3316,7 +3475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -3511,7 +3670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -3592,7 +3751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3636,11 +3795,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -3655,7 +3814,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>238</v>
       </c>
       <c r="C1" s="31" t="s">
@@ -3672,13 +3831,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="35"/>
+      <c r="A3" s="34"/>
     </row>
     <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>242</v>
       </c>
       <c r="D4" s="31" t="s">
@@ -3756,7 +3915,7 @@
       <c r="A17" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>153</v>
       </c>
       <c r="D17" s="31" t="s">
@@ -3777,7 +3936,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="171" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B19" s="30" t="s">
         <v>244</v>
       </c>
@@ -3835,13 +3994,13 @@
       <c r="A26" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="34"/>
+      <c r="C26" s="33"/>
     </row>
     <row r="27" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B27" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="33" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3915,7 +4074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -3976,7 +4135,7 @@
       <c r="B5" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="39" t="s">
         <v>325</v>
       </c>
     </row>
@@ -3987,7 +4146,7 @@
       <c r="B6" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="40" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3997,7 +4156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -4117,7 +4276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4313,8 +4472,8 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F19" s="40"/>
-      <c r="G19" s="41"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
       <c r="H19" t="s">
         <v>185</v>
       </c>
@@ -4323,8 +4482,8 @@
       <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
       <c r="H20" t="s">
         <v>186</v>
       </c>
@@ -4333,8 +4492,8 @@
       <c r="A21" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
@@ -4379,29 +4538,100 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7E12AB-E4A5-4E7D-8358-B6EFAAEDEE14}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="77.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="77.3984375" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A1" s="31" t="s">
+        <v>337</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="31" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="31" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B16:B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="63.796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="63.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="41" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -4409,11 +4639,11 @@
     <hyperlink ref="A1" location="Catalogue!A1" display="Catalogue!A1" xr:uid="{09120829-11D9-4BDC-859E-3D1F07DF5681}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -4441,7 +4671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -4644,12 +4874,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4763,13 +4993,21 @@
         <v>204</v>
       </c>
     </row>
+    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -4819,7 +5057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -4860,79 +5098,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="11.53125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.73046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="65.6640625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="3" spans="1:3" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" location="Catalogue!A1" display="Sorting" xr:uid="{3267D2FA-DC3A-41D3-A13F-612768D8DED2}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Definition of DP
</commit_message>
<xml_diff>
--- a/RunningNotes.xlsx
+++ b/RunningNotes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E0AEC6-4CE9-45F7-948B-D956025378EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E6F650-0A76-4713-953C-7156455112AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="936" firstSheet="3" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1587,94 +1587,11 @@
     <t>Null Object</t>
   </si>
   <si>
-    <t>The adapter is the solution for classes that do similar jobs but don't have a unified interface. Adapter provides the uniform interface and can be implemented using either multiple inheritance or delegation through embedding a member of the adaptee.
-There are two types of Adapter
-1. Objects Adapters(Composition): Adapter Implements the interface. Adapter holds the object of the other class(Adaptee)
-2. Class Adapters (Inheritance): Adapter Implements the interface. Adapter inherits the other class(Adaptee).</t>
-  </si>
-  <si>
     <t>You should consider using the Adapter Pattern whenever you want to use an existing class’s functionality, but its interface is not the one that you require.
 Interfaces are incompatible, but the inner functionality should be as required.
 Decorator and Adapter does wrap already existing object, and such is typically provided in the constructor.
 dzone.com/articles/adapter-design-pattern-in-java
 Decorator and Adapter wrap existing object, and that is typically provided in the constructor.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There are 3 entites in Decorator pattern.
-1. The basic Interface.
-2. One or many concrete Class that provide the basic functionalities.
-3. Decorator Class/Classes that takes/wraps the concrete class(as a construtor argument) and provides the addition functionalities. 
-   The Decorator class should implement the basic interface too(Why---It wil be easy to Use the basic Interface reference and call the operations)
-Decorators should not be inter dependable
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DrawBacks</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.All methods in the decorated interface must be implemented in the decorator class.Can this drawback be solved by combining the command pattern. i.e the Decorators should implement command pattern. May be possible in specific case.
-Or may be create a abstract base class for all the Decorator classes.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Only  good if there are many decorators</t>
-    </r>
   </si>
   <si>
     <t>Coupling</t>
@@ -1833,10 +1750,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Simply speaking, a Proxy object is one through which we control access to the actual object on which the functionality lies. 
-</t>
-  </si>
-  <si>
     <t>The access to an object should be controlled.
 Additional functionality should be provided when accessing an object.</t>
   </si>
@@ -2013,33 +1926,6 @@
 	1.Reflection
 	2.Dependency Injection</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Slight Modification to the origin pattern</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
-If the observer is created by passing the observable(concrete, so that we can access the methods/getters), we can avoid the notify method's arguments. Observer can fetch the details from the observable object passed during creation.</t>
-    </r>
-  </si>
-  <si>
-    <t>Make sure to deRegsister.Memory loss</t>
   </si>
   <si>
     <t>MVC</t>
@@ -2236,16 +2122,6 @@
 One way of achieving abstraction is by using interfaces.</t>
   </si>
   <si>
-    <t xml:space="preserve">Adapters are used when we encounter a problem but Bridge is implemented to avoid futuristic problems.A bridge is by design,put in place on purpose. An adaptor is a patch.
-Separetes the Platform independent from platform dependent.It's the solution whenever there are two orthogonal dimensions in the domain.
-allows loose coupling between algorithm and platform
---&gt;what is the difference between decorator and bridge.Why can't we have multiple decorators 
---&gt;Is Bridge pattern is a composite of the Template and Strategy patterns.
---&gt;View/Resource is a factory.
-      Is Handler/View/Resorse  ==== a bridge pattern?
-</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2330,59 +2206,6 @@
 	Facade Pattern</t>
   </si>
   <si>
-    <t>Used when there are several types algorithms that can be used to perform particular a task. EX:Sorting.
-https://dzone.com/articles/design-patterns-the-strategy-and-factory-patterns
-A factory pattern is used to create objects of a specific type. A strategy pattern is use to perform an operation (or set of operations) in a particular manner.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">More than one factory is available. Abstracted by an interface
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The Factory Method Pattern defines an interface for creating an object, but lets subclasses decide which class to instantiate. Factory Method lets a class defer instantiation to subclasses.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The definition says, the subclass of the factory decides which class to instantiate. so the logic should be in the subclass(The Concrete Class).
-A factory pattern is used to create objects of a specific type. A strategy pattern is use to perform an operation (or set of operations) in a particular manner.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2446,35 +2269,6 @@
       </rPr>
       <t>.
 By intent,Type of Design Pattern</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Factory of Factories 
-The abstract factory pattern provides a way to encapsulate a group of individual factories
-Provide an interface for creating families of related or dependent objects
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Examples of AF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:https://stackoverflow.com/questions/2280170/why-do-we-need-abstract-factory-design-pattern</t>
     </r>
   </si>
   <si>
@@ -2520,42 +2314,6 @@
 We directly call the static inner class constructor and the chain .Finally we call build() of the static inner class which returns the actual object.
 Perform argument validy check as early as possible, may be when creating the actual object(build()) from the builder object and throw IllegalArgumentException if any state issues. which is also needed in regular constructors.
 Buiding the object with builder pattern is better than using setters of the class. If setters are used we cannot make sure that the all the required variables are set. Since build method is mandatory we are sure that checks are done.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Eager Initialization vs Lazy Initialization</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :
-The double check is done because :The lock is grabbed only if the Singleton instance does not exist, and then the existence of the instance is checked again(because,what if another thread has created the instance while this thread is waiting for the lock) in case another thread passed the first check an instant before the current thread. By this, we intend to avoid the expense of grabbing the lock of the Singleton class every time the method is called(Avoiding method Sync).Anyway this is also not good approach.
-In lazy initialization, Singleton is created only when Object is created. But in early initialization, if anything of that class is accessed the singleton object is created i.e if any other static memeber or static variable.
-In lazy initialization you give a public API to get the instance. In multi-threaded environment it is challenging to avoid unnecessary object creation. So we put synchronization blocks which poses unnecessary locking to be done to check for object already created. So it becomes a performance issue in this case.In reality most use cases this sort of code it will always be executed, so is it worth to handle this overhead of thread issues? 
-So if we are sure that creating object is not going to take any significant memory and its almost always going to be used in your application then its good to create in static initialization. Also please do not forget to make your instance final in this case as it make sures that the object creation is reflected properly and in totality to main memory which is important in multi-threaded environment.
-public class BillPughSingleton {
-    private BillPughSingleton(){}
-    private static class SingletonHelper{
-        private static final BillPughSingleton INSTANCE = new BillPughSingleton(); 
-    }
-    public static BillPughSingleton getInstance(){
-        return SingletonHelper.INSTANCE;
-    }
-}</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2739,7 +2497,611 @@
     <t>Interview</t>
   </si>
   <si>
-    <t>Command Pattern intends to encapsulate in an object all the data required for performing a given action (command), including what method to call, the method's arguments, and the object to which the method belongs.
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Members</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:Invoker,command,receiver
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UseCases:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+In some cases, the invoker also stores and queues commands, besides executing them. This is useful for implementing some additional features, undo/redo functionality.
+Are the commands supposed to do some preProcessing/PostProcessing before/after invoking the Receiver? If not, why is the invoker calling the command.Cant it directly call receiver. Yes, pre and post work may be someting like dataBase open and close
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>undo/Redo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :
+Use 2 stacks, undo and redo stack. If you undo an action, it pops from the undo stack and pushes onto the redo stack. Adding a new action is pushing a new one onto the undo stack and clearing the redo stack
+https://stackoverflow.com/questions/1154935/command-pattern-returning-status
+...................understan: Command pattern using generic parameters</t>
+    </r>
+  </si>
+  <si>
+    <t>Helps a lot in Unit testing. We can inject mocked object.
+https://martinfowler.com/articles/injection.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The UML of strategy pattern is same as interfaces &amp; Concrete Class. 
+The UML of Template is similar to Abstract class
+Java has the concept of Abstract class but other languages might does not have.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1. Tax computing website, they ask if we have any investment,HRA...And then calculate
+2. WebPage template</t>
+    </r>
+  </si>
+  <si>
+    <t>Map is not Iterable and it is not a collection.</t>
+  </si>
+  <si>
+    <t>Create a Iterator  to iterate custom objects</t>
+  </si>
+  <si>
+    <t>Build Amazon filters  ,builder pattern</t>
+  </si>
+  <si>
+    <t>Branch Prediction</t>
+  </si>
+  <si>
+    <t>forEachRemaining()</t>
+  </si>
+  <si>
+    <t>Processing a sorted array id faster than unSorted.
+https://stackoverflow.com/questions/11227809/why-is-processing-a-sorted-array-faster-than-processing-an-unsorted-array/11227902#11227902</t>
+  </si>
+  <si>
+    <t>Stream API</t>
+  </si>
+  <si>
+    <t>people.stream().filter(person -&gt; person.getBirthYear() == 1980).forEach(person -&gt; System.out.println(person.getName() + " was born in 1980"));
+people.stream().filter(person -&gt; person.getBirthYear() == 1980).filter(person -&gt; "New York".equals(person.getAddress().getCity())).collect(Collectors.toSet());</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iterating on Maps:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://www.sergiy.ca/how-to-iterate-over-a-map-in-java</t>
+    </r>
+  </si>
+  <si>
+    <t>An interface which tells that the collection is iterable. And to Iterate that collection we can get the Iterator using the methods Iterator().
+The forEach() provides each way to iterate.
+It provides a commom inteface .</t>
+  </si>
+  <si>
+    <t>Map interface does not implement Iterable</t>
+  </si>
+  <si>
+    <t>It has 3 methods.hasNext(), next(), remove().
+By default remove() throws UnsupportedOperationException.
+We can have multiple Iterator for the same Aggretate Object to have diffrerent kind of traversing.</t>
+  </si>
+  <si>
+    <t>wqeqw</t>
+  </si>
+  <si>
+    <t>Code an example of State Pattern:
+Game. Make the character to walk,talk,run,fight. Pass command and change the state. Change state A-&gt; B, A-&gt;A</t>
+  </si>
+  <si>
+    <t>Class and instance variable should be final.
+Constructors should perform deep copy.
+No setters, Getters should return a depy copy of instance variable.
+Primitives,String,Integer etc are immutable</t>
+  </si>
+  <si>
+    <t>Cool Concepts</t>
+  </si>
+  <si>
+    <t>Thread in General</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Volatile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> variables are always read/written from/to the main memory(not from CPU cache or CPU registers).
+More time consuming becuase cache memory cant be used.
+If the  variable is always updated then its okay to use volatile. If the variable is conditionally updated, then race condition comes into picture . So the synchronized code should be used.
+Accessing volatile variables also prevent instruction reordering which is a normal performance enhancement technique.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multitasking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Ability to execute more than one task at the same time is known as multitasking.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multithreading</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: We already discussed about it. It is a process of executing multiple threads simultaneously. Multithreading is also known as Thread-based Multitasking.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multiprocessing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: It is same as multitasking, however in multiprocessing more than one CPUs are involved. On the other hand one CPU is involved in multitasking.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parallel Processing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: It refers to the utilization of multiple CPUs in a single computer system.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A synchronized block guarantees that only one thread can enter a given critical section of the code at any given time.
+Synchronized blocks also guarantee that all variables accessed inside the synchronized block will be read </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in from main memory</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and when the thread exits the synchronized block, all updated variables will be flushed back to main memory again, regardless of whether the variable is declared volatile or not</t>
+    </r>
+  </si>
+  <si>
+    <t>stack/heap/Ram/CPU Cache/CPU registers</t>
+  </si>
+  <si>
+    <t>Stream class and APIs</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Boot Strap</t>
+  </si>
+  <si>
+    <t>JVM</t>
+  </si>
+  <si>
+    <t>Interface with method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JVM </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> memory areas allocated by JVM:Classloader, Class area, Heap, Stack, Program Counter Register and Native Method Stack</t>
+  </si>
+  <si>
+    <t>Why Type Casting is bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In logarithm graph time curve decelerates as n increases.
+https://stackoverflow.com/questions/2307283/what-does-olog-n-mean-exactlyIn
+Logarithm is essentially the inverse of exponentiation.
+Now, if you can prove, that at every iteration of your algorithm you cut off a fraction of this space,
+ that is no less than some limit, this means that your algorithm is running in O(logN) time.
+O(log n) running times are very common in any sort of divide-and-conquer application, because you are (ideally) cutting the work in half every time.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Use factory pattern to return one of many different types of Iterators based on some condition.
+Iterators can be implemented in 2 ways:
+1.Works on the original copy of the collection. This could case runtime exception(CurrentModification) when the someone modifies the collection while Iterating.
+2. Works on a copy of collection to avoid the above problem.But may have stale data.
+3. Or work on original collection and listen to the modification of the collection and update accordingly 
+javapapers.com/design-patterns/iterator-design-pattern/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>STB example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 
+	Program banner and complete Event list. At a given point in time the program banner needs to know only one event data. It needs to know if the next and previous event exists . So iterator is the best .
+Code this banner Iterator to understand better.</t>
+    </r>
+  </si>
+  <si>
+    <t>The Observer Pattern defines a one-to-many dependency between objects so that when one object changes state, all of its dependents are notified and updated automatically.</t>
+  </si>
+  <si>
+    <t>Make sure to deRegsister.Memory loss.
+Slight Modification to the origin pattern:
+If the observer is created by passing the observable(concrete, so that we can access the methods/getters), we can avoid the notify method's arguments. Observer can fetch the details from the observable object passed during creation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Decorator Pattern attaches additional responsibilities to an object dynamically. Decorators provide a flexible alternative to subclassing for extending functionality.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+There are 3 entites in Decorator pattern.
+1. The basic Interface.
+2. One or many concrete Class that provide the basic functionalities.
+3. Decorator Class/Classes that takes/wraps the concrete class(as a construtor argument) and provides the addition functionalities. 
+   The Decorator class should implement the basic interface too(Why---It wil be easy to Use the basic Interface reference and call the operations)
+Decorators should not be inter dependable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DrawBacks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.All methods in the decorated interface must be implemented in the decorator class.Can this drawback be solved by combining the command pattern. i.e the Decorators should implement command pattern. May be possible in specific case.
+Or may be create a abstract base class for all the Decorator classes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Only  good if there are many decorators</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Factory Method Pattern defines an interface for creating an object, but lets subclasses decide which class to instantiate. Factory Method lets a class defer instantiation to subclasses.
+More than one factory is available. Abstracted by an interface
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Factory Method Pattern defines an interface for creating an object, but lets subclasses decide which class to instantiate. Factory Method lets a class defer instantiation to subclasses.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The definition says, the subclass of the factory decides which class to instantiate. so the logic should be in the subclass(The Concrete Class).
+A factory pattern is used to create objects of a specific type. A strategy pattern is use to perform an operation (or set of operations) in a particular manner.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Singleton Pattern ensures a class has only one instance, and provides a global point of access to it.
+Eager Initialization vs Lazy Initialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :
+The double check is done because :The lock is grabbed only if the Singleton instance does not exist, and then the existence of the instance is checked again(because,what if another thread has created the instance while this thread is waiting for the lock) in case another thread passed the first check an instant before the current thread. By this, we intend to avoid the expense of grabbing the lock of the Singleton class every time the method is called(Avoiding method Sync).Anyway this is also not good approach.
+In lazy initialization, Singleton is created only when Object is created. But in early initialization, if anything of that class is accessed the singleton object is created i.e if any other static memeber or static variable.
+In lazy initialization you give a public API to get the instance. In multi-threaded environment it is challenging to avoid unnecessary object creation. So we put synchronization blocks which poses unnecessary locking to be done to check for object already created. So it becomes a performance issue in this case.In reality most use cases this sort of code it will always be executed, so is it worth to handle this overhead of thread issues? 
+So if we are sure that creating object is not going to take any significant memory and its almost always going to be used in your application then its good to create in static initialization. Also please do not forget to make your instance final in this case as it make sures that the object creation is reflected properly and in totality to main memory which is important in multi-threaded environment.
+public class BillPughSingleton {
+    private BillPughSingleton(){}
+    private static class SingletonHelper{
+        private static final BillPughSingleton INSTANCE = new BillPughSingleton(); 
+    }
+    public static BillPughSingleton getInstance(){
+        return SingletonHelper.INSTANCE;
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Command Pattern encapsulates a request as an object, thereby letting you parameterize other objects with different requests, queue or log requests, and support undoable operations.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Command Pattern intends to encapsulate in an object all the data required for performing a given action (command), including what method to call, the method's arguments, and the object to which the method belongs.
 The pattern encapsulates everything required to take an action and allows the execution of the action to occur completely independently of any of that context. If that is not a requirement for you then the pattern is probably not helpful for your problem space
 They can have parameterised constructor but is it possible to know the parameters at the time of command creation ?
 Returning the result : 
@@ -2747,40 +3109,19 @@
 1. Either by observer pattern 
 2. the invoker object passing a Result object as a argument to the method call so that command or Receiver object loading the result.
 Even though it is possible to pass arguments and return value from command, it is not recommanded because they are supposed to work independently.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Members</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:Invoker,command,receiver
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>UseCases:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Adapter Pattern converts the interface of a class into another interface the clients expect. Adapter lets classes work together that couldn’t otherwise because of incompatible interfaces.</t>
     </r>
     <r>
       <rPr>
@@ -2791,73 +3132,34 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-In some cases, the invoker also stores and queues commands, besides executing them. This is useful for implementing some additional features, undo/redo functionality.
-Are the commands supposed to do some preProcessing/PostProcessing before/after invoking the Receiver? If not, why is the invoker calling the command.Cant it directly call receiver. Yes, pre and post work may be someting like dataBase open and close
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>undo/Redo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :
-Use 2 stacks, undo and redo stack. If you undo an action, it pops from the undo stack and pushes onto the redo stack. Adding a new action is pushing a new one onto the undo stack and clearing the redo stack
-https://stackoverflow.com/questions/1154935/command-pattern-returning-status
-...................understan: Command pattern using generic parameters</t>
-    </r>
-  </si>
-  <si>
-    <t>Helps a lot in Unit testing. We can inject mocked object.
-https://martinfowler.com/articles/injection.html</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The UML of strategy pattern is same as interfaces &amp; Concrete Class. 
-The UML of Template is similar to Abstract class
-Java has the concept of Abstract class but other languages might does not have.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Example:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-1. Tax computing website, they ask if we have any investment,HRA...And then calculate
-2. WebPage template</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Members: Abstract class and it concrete class !!
+The adapter is the solution for classes that do similar jobs but don't have a unified interface. Adapter provides the uniform interface and can be implemented using either multiple inheritance or delegation through embedding a member of the adaptee.
+There are two types of Adapter
+1. Objects Adapters(Composition): Adapter Implements the interface. Adapter holds the object of the other class(Adaptee)
+2. Class Adapters (Inheritance): Adapter Implements the interface. Adapter inherits the other class(Adaptee).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Template Method Pattern defines the skeleton of an algorithm in a method, deferring some steps to subclasses. Template Method lets subclasses redefine certain steps of an algorithm without changing the algorithm’s structure.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Members: Abstract class and it concrete class !!
 The Template Method Pattern defines the skeleton of an algorithm in a method, deferring some steps to subclasses. Template Method lets subclasses redefine certain steps of an algorithm without changing the algorithm’s structure.
 The template method is declared </t>
     </r>
@@ -2884,261 +3186,27 @@
     </r>
   </si>
   <si>
-    <t>Map is not Iterable and it is not a collection.</t>
-  </si>
-  <si>
-    <t>Create a Iterator  to iterate custom objects</t>
-  </si>
-  <si>
-    <t>Build Amazon filters  ,builder pattern</t>
-  </si>
-  <si>
-    <t>Branch Prediction</t>
-  </si>
-  <si>
-    <t>forEachRemaining()</t>
-  </si>
-  <si>
-    <t>Processing a sorted array id faster than unSorted.
-https://stackoverflow.com/questions/11227809/why-is-processing-a-sorted-array-faster-than-processing-an-unsorted-array/11227902#11227902</t>
-  </si>
-  <si>
-    <t>Stream API</t>
-  </si>
-  <si>
-    <t>people.stream().filter(person -&gt; person.getBirthYear() == 1980).forEach(person -&gt; System.out.println(person.getName() + " was born in 1980"));
-people.stream().filter(person -&gt; person.getBirthYear() == 1980).filter(person -&gt; "New York".equals(person.getAddress().getCity())).collect(Collectors.toSet());</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Iterating on Maps:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>http://www.sergiy.ca/how-to-iterate-over-a-map-in-java</t>
-    </r>
-  </si>
-  <si>
-    <t>An interface which tells that the collection is iterable. And to Iterate that collection we can get the Iterator using the methods Iterator().
-The forEach() provides each way to iterate.
-It provides a commom inteface .</t>
-  </si>
-  <si>
-    <t>Map interface does not implement Iterable</t>
-  </si>
-  <si>
-    <t>It has 3 methods.hasNext(), next(), remove().
-By default remove() throws UnsupportedOperationException.
-We can have multiple Iterator for the same Aggretate Object to have diffrerent kind of traversing.</t>
-  </si>
-  <si>
-    <t>wqeqw</t>
-  </si>
-  <si>
-    <t>Code an example of State Pattern:
-Game. Make the character to walk,talk,run,fight. Pass command and change the state. Change state A-&gt; B, A-&gt;A</t>
-  </si>
-  <si>
-    <t>Class and instance variable should be final.
-Constructors should perform deep copy.
-No setters, Getters should return a depy copy of instance variable.
-Primitives,String,Integer etc are immutable</t>
-  </si>
-  <si>
-    <t>Cool Concepts</t>
-  </si>
-  <si>
-    <t>Thread in General</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Volatile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> variables are always read/written from/to the main memory(not from CPU cache or CPU registers).
-More time consuming becuase cache memory cant be used.
-If the  variable is always updated then its okay to use volatile. If the variable is conditionally updated, then race condition comes into picture . So the synchronized code should be used.
-Accessing volatile variables also prevent instruction reordering which is a normal performance enhancement technique.
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Multitasking</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: Ability to execute more than one task at the same time is known as multitasking.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Multithreading</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: We already discussed about it. It is a process of executing multiple threads simultaneously. Multithreading is also known as Thread-based Multitasking.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Multiprocessing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: It is same as multitasking, however in multiprocessing more than one CPUs are involved. On the other hand one CPU is involved in multitasking.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Parallel Processing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: It refers to the utilization of multiple CPUs in a single computer system.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A synchronized block guarantees that only one thread can enter a given critical section of the code at any given time.
-Synchronized blocks also guarantee that all variables accessed inside the synchronized block will be read </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>in from main memory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and when the thread exits the synchronized block, all updated variables will be flushed back to main memory again, regardless of whether the variable is declared volatile or not</t>
-    </r>
-  </si>
-  <si>
-    <t>stack/heap/Ram/CPU Cache/CPU registers</t>
-  </si>
-  <si>
-    <t>Stream class and APIs</t>
-  </si>
-  <si>
-    <t>Git</t>
-  </si>
-  <si>
-    <t>Boot Strap</t>
-  </si>
-  <si>
-    <t>JVM</t>
-  </si>
-  <si>
-    <t>Interface with method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JVM </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> memory areas allocated by JVM:Classloader, Class area, Heap, Stack, Program Counter Register and Native Method Stack</t>
-  </si>
-  <si>
-    <t>Why Type Casting is bad</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> In logarithm graph time curve decelerates as n increases.
-https://stackoverflow.com/questions/2307283/what-does-olog-n-mean-exactlyIn
-Logarithm is essentially the inverse of exponentiation.
-Now, if you can prove, that at every iteration of your algorithm you cut off a fraction of this space,
- that is no less than some limit, this means that your algorithm is running in O(logN) time.
-O(log n) running times are very common in any sort of divide-and-conquer application, because you are (ideally) cutting the work in half every time.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Iterator Pattern provides a way to access the elements(seguentially ?) of an aggregate object without exposing the underlying structure.
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Iterator Pattern provides a way to access the elements of an aggregate object sequentially without exposing its underlying representation.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Iterator Pattern provides a way to access the elements(seguentially ?) of an aggregate object without exposing the underlying structure.
 with Iterator pattern, we should be able to Iterator in any aggregation of Objects. Ex: List Employee objects
 What is the need of Iterable intertace,Why cant we directly get the iterator? 
 Imagine Iterable inteface is not there. so to get the iterator of (say) Employee::getEmployeeIterator(), Student::getStudentlterator(), getTeacherlterator(). So Iterable provides a unified API. 
@@ -3175,44 +3243,161 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Use factory pattern to return one of many different types of Iterators based on some condition.
-Iterators can be implemented in 2 ways:
-1.Works on the original copy of the collection. This could case runtime exception(CurrentModification) when the someone modifies the collection while Iterating.
-2. Works on a copy of collection to avoid the above problem.But may have stale data.
-3. Or work on original collection and listen to the modification of the collection and update accordingly 
-javapapers.com/design-patterns/iterator-design-pattern/
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>STB example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 
-	Program banner and complete Event list. At a given point in time the program banner needs to know only one event data. It needs to know if the next and previous event exists . So iterator is the best .
-Code this banner Iterator to understand better.</t>
-    </r>
-  </si>
-  <si>
-    <t>The State Pattern allows an object to alter its behavior when its internal state changes.
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The State Pattern allows an object to alter its behavior when its internal state changes. The object will appear to change its class.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The State Pattern allows an object to alter its behavior when its internal state changes.
 When the concrete state object about to set the next state , it is better NOT to set the state(constant or new StateObject() directly . Instead use the help of factory or some kind of dependence injection to avoid class coupling
 Ex: to set the nextstate : getProcessingState() 
 Stratergy and state have similar UML.
 State Machine is different from state design pattern</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Proxy Pattern provides a surrogate or placeholder for another object to control access to it.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Simply speaking, a Proxy object is one through which we control access to the actual object on which the functionality lies. 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Strategy Pattern defines a family of algorithms, encapsulates each one, and makes them interchangeable. Strategy lets the algorithm vary independently from clients that use it.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Used when there are several types algorithms that can be used to perform particular a task. EX:Sorting.
+https://dzone.com/articles/design-patterns-the-strategy-and-factory-patterns
+A factory pattern is used to create objects of a specific type. A strategy pattern is use to perform an operation (or set of operations) in a particular manner.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Decouple an abstraction from its implementation so that the two can vary independently.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Adapters are used when we encounter a problem but Bridge is implemented to avoid futuristic problems.A bridge is by design,put in place on purpose. An adaptor is a patch.
+Separetes the Platform independent from platform dependent.It's the solution whenever there are two orthogonal dimensions in the domain.
+allows loose coupling between algorithm and platform
+--&gt;what is the difference between decorator and bridge.Why can't we have multiple decorators 
+--&gt;Is Bridge pattern is a composite of the Template and Strategy patterns.
+--&gt;View/Resource is a factory.
+      Is Handler/View/Resorse  ==== a bridge pattern?
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Abstract Factory Pattern provides an interface for creating families of related or dependent objects without specifying their concrete classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Factory of Factories 
+The abstract factory pattern provides a way to encapsulate a group of individual factories
+Provide an interface for creating families of related or dependent objects
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Examples of AF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:https://stackoverflow.com/questions/2280170/why-do-we-need-abstract-factory-design-pattern</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3823,7 +4008,7 @@
         <v>170</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -3832,7 +4017,7 @@
         <v>36</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -3857,7 +4042,7 @@
         <v>139</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I7" s="26" t="s">
         <v>76</v>
@@ -3871,7 +4056,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="26"/>
       <c r="G9" s="26" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -3954,7 +4139,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C3" s="16" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -4017,12 +4202,12 @@
     </row>
     <row r="19" spans="4:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D19" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="D21" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -4095,7 +4280,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4304,80 +4489,80 @@
         <v>148</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G18" s="34"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F19" s="30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="57" x14ac:dyDescent="0.45">
       <c r="F20" s="30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F21" s="30" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G21" s="30"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F22" s="30" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F23" s="30" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F24" s="30" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F25" s="30" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F26" s="30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G26" s="30"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.45">
       <c r="F27" s="30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G27" s="30"/>
     </row>
     <row r="29" spans="2:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="G29" s="30" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="142.5" x14ac:dyDescent="0.45">
       <c r="G30" s="30" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -4468,7 +4653,7 @@
         <v>68</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
@@ -4476,7 +4661,7 @@
         <v>66</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
@@ -4484,7 +4669,7 @@
         <v>67</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -4502,7 +4687,7 @@
         <v>239</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="57" x14ac:dyDescent="0.45">
@@ -4510,7 +4695,7 @@
         <v>237</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
@@ -4518,7 +4703,7 @@
         <v>238</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
@@ -4570,20 +4755,20 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="29" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="29" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B35" s="30" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -4678,10 +4863,10 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="6" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4752,8 +4937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4771,25 +4956,25 @@
         <v>221</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
       <c r="C2" s="30" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="33"/>
       <c r="B3" s="28" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -4805,79 +4990,79 @@
     </row>
     <row r="5" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B5" s="29" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B6" s="29" t="s">
         <v>108</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B7" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>288</v>
+      <c r="C7" s="32" t="s">
+        <v>364</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="270.75" x14ac:dyDescent="0.45">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B8" s="29" t="s">
         <v>103</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>340</v>
+        <v>369</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="285" x14ac:dyDescent="0.45">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B9" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B10" s="29" t="s">
         <v>109</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>344</v>
+        <v>371</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B11" s="29" t="s">
         <v>107</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -4895,12 +5080,12 @@
         <v>105</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15" s="28" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="57" x14ac:dyDescent="0.45">
@@ -4911,7 +5096,7 @@
         <v>141</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
@@ -4919,24 +5104,24 @@
         <v>111</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>251</v>
+        <v>366</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B19" s="29" t="s">
         <v>227</v>
       </c>
       <c r="C19" s="30" t="s">
+        <v>370</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>249</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="285" x14ac:dyDescent="0.45">
@@ -4944,10 +5129,10 @@
         <v>229</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>314</v>
+        <v>376</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
@@ -4955,21 +5140,21 @@
         <v>228</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B22" s="29" t="s">
         <v>222</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>276</v>
+        <v>374</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -4990,32 +5175,32 @@
     </row>
     <row r="27" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B27" s="28" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="171" x14ac:dyDescent="0.45">
       <c r="B28" s="29" t="s">
         <v>112</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>319</v>
+        <v>367</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B29" s="29" t="s">
         <v>231</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>325</v>
+        <v>377</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="409.5" x14ac:dyDescent="0.45">
@@ -5023,10 +5208,10 @@
         <v>115</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>332</v>
+        <v>368</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="213.75" x14ac:dyDescent="0.45">
@@ -5034,10 +5219,10 @@
         <v>113</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -5047,7 +5232,7 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="29" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
@@ -5057,7 +5242,7 @@
     </row>
     <row r="40" spans="1:1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -5090,7 +5275,7 @@
         <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
@@ -5101,7 +5286,7 @@
         <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="171" x14ac:dyDescent="0.45">
@@ -5109,10 +5294,10 @@
         <v>128</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
@@ -5120,7 +5305,7 @@
         <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>240</v>
@@ -5131,21 +5316,21 @@
         <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5341,7 +5526,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -5357,7 +5542,7 @@
         <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -5365,7 +5550,7 @@
         <v>122</v>
       </c>
       <c r="E11" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -5426,7 +5611,7 @@
         <v>121</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -5434,12 +5619,12 @@
         <v>124</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E23" s="7" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -5447,10 +5632,10 @@
     </row>
     <row r="40" spans="1:2" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A40" s="8" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -5481,10 +5666,10 @@
     </row>
     <row r="2" spans="1:3" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -5494,7 +5679,7 @@
     </row>
     <row r="4" spans="1:3" ht="114" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
@@ -5534,10 +5719,10 @@
     </row>
     <row r="3" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -5568,23 +5753,23 @@
     </row>
     <row r="2" spans="1:3" ht="242.25" x14ac:dyDescent="0.45">
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="199.5" x14ac:dyDescent="0.45">
       <c r="B3" s="30" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="30" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -5628,37 +5813,37 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="30" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="30" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B8" s="30" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="57" x14ac:dyDescent="0.45">
       <c r="B10" s="30" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B11" s="30" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" s="30" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" s="30" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -5696,7 +5881,7 @@
         <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -5706,12 +5891,12 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5750,7 +5935,7 @@
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="39"/>
       <c r="B2" s="1" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -5778,10 +5963,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="57" x14ac:dyDescent="0.45">
@@ -5789,7 +5974,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -5854,7 +6039,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -5931,7 +6116,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -6001,10 +6186,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="256.5" x14ac:dyDescent="0.45">
@@ -6023,7 +6208,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>126</v>
@@ -6099,7 +6284,7 @@
     </row>
     <row r="3" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>